<commit_message>
Après le lunch - 2023-12-15
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_DB_Sortie.xlsx
+++ b/DataFiles/GCF_DB_Sortie.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBA\GC_FISCALITÉ\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0A44BC-C4B9-427C-BE66-577859B50A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD489AE-6EF8-454A-B670-1DABDE882892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="TEC" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,137 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+  <si>
+    <t>TEC_ID</t>
+  </si>
+  <si>
+    <t>Prof_ID</t>
+  </si>
+  <si>
+    <t>Prof</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Client_ID</t>
+  </si>
+  <si>
+    <t>ClientNom</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Heures</t>
+  </si>
+  <si>
+    <t>CommentaireNote</t>
+  </si>
+  <si>
+    <t>EstFacturable</t>
+  </si>
+  <si>
+    <t>DateSaisie</t>
+  </si>
+  <si>
+    <t>EstFacturee</t>
+  </si>
+  <si>
+    <t>DateFacturee</t>
+  </si>
+  <si>
+    <t>EstDetruit</t>
+  </si>
+  <si>
+    <t>VersionApp</t>
+  </si>
+  <si>
+    <t>NoFacture</t>
+  </si>
+  <si>
+    <t>GC</t>
+  </si>
+  <si>
+    <t>15/déc/2023</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>ABB LTD</t>
+  </si>
+  <si>
+    <t>Test d'écriture dans la BD externe</t>
+  </si>
+  <si>
+    <t>0,25</t>
+  </si>
+  <si>
+    <t>15/déc/2023 11:04:18</t>
+  </si>
+  <si>
+    <t>v1.0.3</t>
+  </si>
+  <si>
+    <t>RMV</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>Gestion ABCD inc.</t>
+  </si>
+  <si>
+    <t>Test avec le ID du fichier externe</t>
+  </si>
+  <si>
+    <t>1,00</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>15/déc/2023 11:11:17</t>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>Jack In The Box Inc.</t>
+  </si>
+  <si>
+    <t>Test with ADO - Écriture dans fichier fermé</t>
+  </si>
+  <si>
+    <t>15/déc/2023 12:52:33</t>
+  </si>
+  <si>
+    <t>Test # 2</t>
+  </si>
+  <si>
+    <t>0,50</t>
+  </si>
+  <si>
+    <t>15/déc/2023 12:54:23</t>
+  </si>
+  <si>
+    <t>1134</t>
+  </si>
+  <si>
+    <t>Marie Guay, experte en RH</t>
+  </si>
+  <si>
+    <t>Planification de base</t>
+  </si>
+  <si>
+    <t>2,00</t>
+  </si>
+  <si>
+    <t>15/déc/2023 12:57:04</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -61,15 +191,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -77,24 +219,86 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -377,81 +581,289 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="7" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="24.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C2" s="5"/>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="5"/>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" s="5"/>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" s="5"/>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="5"/>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Après les courses au village - 2023-12-15
</commit_message>
<xml_diff>
--- a/DataFiles/GCF_DB_Sortie.xlsx
+++ b/DataFiles/GCF_DB_Sortie.xlsx
@@ -579,11 +579,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -607,7 +607,7 @@
     <col min="16" max="16" width="10.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -657,7 +657,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -698,7 +698,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="3">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -742,7 +742,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="4">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -783,7 +783,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="5">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -824,7 +824,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row spans="1:16" x14ac:dyDescent="0.25" outlineLevel="0" r="6">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -863,6 +863,63 @@
       </c>
       <c r="O6" s="2" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="16">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16">
+        <v>4</v>
+      </c>
+      <c r="C7" s="16" t="inlineStr">
+        <is>
+          <t>RMV</t>
+        </is>
+      </c>
+      <c r="D7" s="16" t="inlineStr">
+        <is>
+          <t>15/déc/2023</t>
+        </is>
+      </c>
+      <c r="E7" s="16" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="F7" s="16" t="inlineStr">
+        <is>
+          <t>Adecco SA</t>
+        </is>
+      </c>
+      <c r="G7" s="16" t="inlineStr">
+        <is>
+          <t>Test de validité des données</t>
+        </is>
+      </c>
+      <c r="H7" s="16" t="inlineStr">
+        <is>
+          <t>0,50</t>
+        </is>
+      </c>
+      <c r="J7" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="16" t="inlineStr">
+        <is>
+          <t>15/déc/2023 13:27:18</t>
+        </is>
+      </c>
+      <c r="L7" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" s="16" t="inlineStr">
+        <is>
+          <t>v1.0.3</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>